<commit_message>
Final_version of Add/Detect using 2 paratmeters
Few bugs are sorted out from the previous file
</commit_message>
<xml_diff>
--- a/Source_file_sl/gesture2.xlsx
+++ b/Source_file_sl/gesture2.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
@@ -508,6 +508,22 @@
         <v>54.85889058807174</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>6</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> five</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="n">
+        <v>53.95540475036354</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>